<commit_message>
cleaned up links, added comments column
</commit_message>
<xml_diff>
--- a/documentation/order_list_V3.xlsx
+++ b/documentation/order_list_V3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonvalov/Documents/mice_task/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konstantinbakhurin/Documents/Writing/Control task in mice/Self-taught/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A1DBDC9-5A08-5A4C-8427-AAF147602211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC959E64-B315-D446-8F54-B56331BFD158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16020" xr2:uid="{8B91018B-20F9-CD43-AEE4-527951079336}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Order List</t>
   </si>
@@ -53,15 +53,9 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://www.amazon.com/WWZMDiB-ADS1115-Converter-Raspberry-Experiments/dp/B0C8JFZ3D9/ref=sr_1_3_pp?crid=1KSNZ7G6TFHL2&amp;dib=eyJ2IjoiMSJ9.j9UEYuVa8hkzdAISJf6vxQV80Cl3S1VscO-wIxlTqbvwhi_JMi5v6tZQlRqnEFSs4NDwCP4iVoqk8mntwZ_iqqOVhEvi7Ane30SlpgSmzbLbCytsgD2pIpVdshmuNy-y4EeWtNK2cZH-9xRRjuBKf0n1TZPg_e4Txim76ZNptbhYlstLBBscu1Y8mqDyTPGfoEvsK_aeHShlP4cn7LQo1j326YPxl8kg69-ehmDPs3Y.bhwmPKeJu9MBdv74ywsAViJwuFFk07i6ZYv4SR0D4vw&amp;dib_tag=se&amp;keywords=ads1115&amp;qid=1744573177&amp;sprefix=ads111%2Caps%2C158&amp;sr=8-3</t>
-  </si>
-  <si>
     <t>WWZMDiB 4Pcs ADS1115 16 Bit 16 Byte 4 Channel I2C IIC Analog-to-Digital ADC PGA Converter for Arduino Raspberry Pi DIY and Other Experiments</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0BSBD669Q?ref=ppx_yo2ov_dt_b_fed_asin_title&amp;th=1</t>
-  </si>
-  <si>
     <t>Rigid Coupling Copper Shaft Coupler Connector Motor Accessories [for 3D Printer]-3mm to 3.17mm Bore L20 x D9/Gold</t>
   </si>
   <si>
@@ -74,15 +68,6 @@
     <t>B0C8JFZ3D9</t>
   </si>
   <si>
-    <t>www.amazon.com/dp/B0824VSF74?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
-  </si>
-  <si>
-    <t>www.amazon.com/dp/B07P6X9M14?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B0B18QWR3L?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
-  </si>
-  <si>
     <t>150mm x 3mm （5.9InchX1/8Inch） 304 Stainless SteelSolid Round Bar Lathe bar Stock. Pack of 20</t>
   </si>
   <si>
@@ -92,9 +77,6 @@
     <t>ASIN</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Easycargo-Raspberry-30x30x7mm-Brushless-30mmx30mmx7mm/dp/B0792BW2VH/ref=sr_1_3?crid=3BKNUC8GSCB4&amp;dib=eyJ2IjoiMSJ9.sQppiE3bTwhEsWO3l_qjZs9Hr9KckjwnOQisHhgp7uUfLBzIXl5ZKDMfqh1laFJBZilCraQpXYDzCOtFebzoIe2U923IYhEDnOLtURRLdtHjBC8ChonZX4g-cDmCHssQiSQvePyg703FZDG1aDCHdKNbOqwwPttzwBxTkXUUQXEA3SXZYB084bhBIIkJ3ztvxxosiZGcrFb3W9ZymshuFS9GIP41fMtRW3e0N4Ev66nyca8-FloXdC22IPD7Ba-eUodSlQNQwYPi-XPwh0Jvfvod1V-u-cvgmHI113R6rmw.zEb1djbNq1oBnkbsaDBDYIixRFH_87hMeYKCWaFjbRE&amp;dib_tag=se&amp;keywords=30mm%2Bfan&amp;qid=1744573755&amp;s=industrial&amp;sprefix=30mm%2Bfan%2B%2Cindustrial%2C128&amp;sr=1-3&amp;th=1</t>
-  </si>
-  <si>
     <t>B0792BW2VH</t>
   </si>
   <si>
@@ -131,13 +113,43 @@
     <t>B01G50OHZM</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0C7776RYQ?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
-  </si>
-  <si>
     <t>100Pcs Spring Probe Round Pogo Conical Head Thimble Testing Pin Contact Replacement for POGOPIN</t>
   </si>
   <si>
     <t>B0C7776RYQ</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>https://a.co/d/iMFugCz</t>
+  </si>
+  <si>
+    <t>https://a.co/d/0P3QT8o</t>
+  </si>
+  <si>
+    <t>the stated size is not a n option</t>
+  </si>
+  <si>
+    <t>unclear which one</t>
+  </si>
+  <si>
+    <t>https://a.co/d/68nAn9N</t>
+  </si>
+  <si>
+    <t>https://a.co/d/3TOCVfs</t>
+  </si>
+  <si>
+    <t>https://a.co/d/fXxFsQx</t>
+  </si>
+  <si>
+    <t>whch one?</t>
+  </si>
+  <si>
+    <t>https://a.co/d/30Kv3W6</t>
+  </si>
+  <si>
+    <t>https://a.co/d/8XVI04L</t>
   </si>
 </sst>
 </file>
@@ -373,6 +385,30 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,13 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -397,24 +427,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -757,10 +769,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9B5FF5-1965-C84C-B5D8-49E66010709B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+      <selection activeCell="J18" sqref="J18:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,445 +780,457 @@
     <col min="8" max="8" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="15" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="18"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="28"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+      <c r="M9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="4">
         <v>15.99</v>
       </c>
-      <c r="J10" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="J10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="1">
         <v>1</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="F11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="5">
         <v>5.99</v>
       </c>
-      <c r="J11" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="25"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="J11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="10"/>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="F12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="4">
         <v>7.99</v>
       </c>
-      <c r="J12" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="27"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="J12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+      <c r="M12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="F13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="5">
         <v>9.99</v>
       </c>
-      <c r="J13" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="J13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="F14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="4">
         <v>8.2899999999999991</v>
       </c>
-      <c r="J14" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="J14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="F15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="5">
         <v>8.69</v>
       </c>
-      <c r="J15" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="J15" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="F16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="4">
         <v>6.99</v>
       </c>
-      <c r="J16" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="27"/>
+      <c r="J16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="B17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+      <c r="F17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="5">
         <v>11.99</v>
       </c>
-      <c r="J17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="25"/>
+      <c r="J17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="B18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="2">
         <v>1</v>
       </c>
-      <c r="F18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="F18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="4">
         <v>34</v>
       </c>
-      <c r="J18" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="27"/>
+      <c r="J18" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="25"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="27"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="25"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="27"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="25"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="27"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="12"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="25"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="4"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="27"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="25"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="10"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="27"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="25"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="10"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="30"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="14"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H31" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I31" s="8">
         <f>SUM(I10:I30)</f>
@@ -1215,16 +1239,49 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="A1:E5"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="J10:L10"/>
@@ -1241,60 +1298,27 @@
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="J8:L9"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="A1:E5"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J23:L23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1" display="https://www.amazon.com/WWZMDiB-ADS1115-Converter-Raspberry-Experiments/dp/B0C8JFZ3D9/ref=sr_1_3_pp?crid=1KSNZ7G6TFHL2&amp;dib=eyJ2IjoiMSJ9.j9UEYuVa8hkzdAISJf6vxQV80Cl3S1VscO-wIxlTqbvwhi_JMi5v6tZQlRqnEFSs4NDwCP4iVoqk8mntwZ_iqqOVhEvi7Ane30SlpgSmzbLbCytsgD2pIpVdshmuNy-y4EeWtNK2cZH-9xRRjuBKf0n1TZPg_e4Txim76ZNptbhYlstLBBscu1Y8mqDyTPGfoEvsK_aeHShlP4cn7LQo1j326YPxl8kg69-ehmDPs3Y.bhwmPKeJu9MBdv74ywsAViJwuFFk07i6ZYv4SR0D4vw&amp;dib_tag=se&amp;keywords=ads1115&amp;qid=1744573177&amp;sprefix=ads111%2Caps%2C158&amp;sr=8-3" xr:uid="{0657F225-79F5-684A-9249-57A0D5149D2A}"/>
-    <hyperlink ref="J11" r:id="rId2" xr:uid="{E07D89ED-4660-B64B-8F49-D38B6DAE2631}"/>
-    <hyperlink ref="J12" r:id="rId3" xr:uid="{17454257-77D6-CB45-99AE-FE91F19FD347}"/>
-    <hyperlink ref="J13" r:id="rId4" display="https://www.amazon.com/Easycargo-Raspberry-30x30x7mm-Brushless-30mmx30mmx7mm/dp/B0792BW2VH/ref=sr_1_3?crid=3BKNUC8GSCB4&amp;dib=eyJ2IjoiMSJ9.sQppiE3bTwhEsWO3l_qjZs9Hr9KckjwnOQisHhgp7uUfLBzIXl5ZKDMfqh1laFJBZilCraQpXYDzCOtFebzoIe2U923IYhEDnOLtURRLdtHjBC8ChonZX4g-cDmCHssQiSQvePyg703FZDG1aDCHdKNbOqwwPttzwBxTkXUUQXEA3SXZYB084bhBIIkJ3ztvxxosiZGcrFb3W9ZymshuFS9GIP41fMtRW3e0N4Ev66nyca8-FloXdC22IPD7Ba-eUodSlQNQwYPi-XPwh0Jvfvod1V-u-cvgmHI113R6rmw.zEb1djbNq1oBnkbsaDBDYIixRFH_87hMeYKCWaFjbRE&amp;dib_tag=se&amp;keywords=30mm%2Bfan&amp;qid=1744573755&amp;s=industrial&amp;sprefix=30mm%2Bfan%2B%2Cindustrial%2C128&amp;sr=1-3&amp;th=1" xr:uid="{535DAD8D-1D12-2840-8E22-3EC117FBAE0D}"/>
-    <hyperlink ref="J14" r:id="rId5" xr:uid="{7603463C-66DD-D749-A4EC-CF8E69D04A85}"/>
-    <hyperlink ref="J15" r:id="rId6" xr:uid="{2240F32A-886E-B849-8901-9B6B2C3D7ABF}"/>
-    <hyperlink ref="J16" r:id="rId7" xr:uid="{7443ABF5-ECC0-834E-A25C-263268CD9C15}"/>
-    <hyperlink ref="J18" r:id="rId8" xr:uid="{883A45C4-C90C-8F4F-B1E4-9DE9323FF356}"/>
-    <hyperlink ref="J17" r:id="rId9" xr:uid="{A776F461-31A5-CF4C-8F90-BE1933DF669C}"/>
+    <hyperlink ref="J18" r:id="rId1" xr:uid="{883A45C4-C90C-8F4F-B1E4-9DE9323FF356}"/>
+    <hyperlink ref="J17" r:id="rId2" xr:uid="{A776F461-31A5-CF4C-8F90-BE1933DF669C}"/>
+    <hyperlink ref="J10" r:id="rId3" xr:uid="{6324F10F-0BF1-9543-975B-E05B43BFEC8F}"/>
+    <hyperlink ref="J11" r:id="rId4" xr:uid="{AE15D379-B474-E449-99DA-2B0022ACA323}"/>
+    <hyperlink ref="J12" r:id="rId5" xr:uid="{300CB9D2-47CF-8C43-9117-B00389709E9E}"/>
+    <hyperlink ref="J13" r:id="rId6" xr:uid="{133D7FA2-DF23-6746-A709-1E9BC8E51BF7}"/>
+    <hyperlink ref="J14" r:id="rId7" xr:uid="{2BC99128-26EE-5146-A766-A21A02A1F0FE}"/>
+    <hyperlink ref="J15" r:id="rId8" xr:uid="{54AAD474-D654-774B-91EB-5EDF340000FE}"/>
+    <hyperlink ref="J16" r:id="rId9" xr:uid="{64AA8519-80F4-2A46-B18D-0CCFF9AE9129}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: fixed order quantities
</commit_message>
<xml_diff>
--- a/documentation/order_list_V3.xlsx
+++ b/documentation/order_list_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konstantinbakhurin/Documents/GitHub/mice_task/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonvalov/Documents/mice_task/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F86E93-E391-4D41-94A1-0E051DABD716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46D46DD5-13DA-6341-BF84-9E8E68B9E9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34840" windowHeight="16020" xr2:uid="{8B91018B-20F9-CD43-AEE4-527951079336}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16020" xr2:uid="{8B91018B-20F9-CD43-AEE4-527951079336}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -386,22 +386,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,10 +413,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -425,23 +425,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,8 +784,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,536 +796,577 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="28" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="20"/>
-      <c r="N8" s="21"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="27"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="23"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="8"/>
       <c r="J10" s="4">
         <v>15.99</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="13">
         <f>J10*E10</f>
         <v>15.99</v>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="39"/>
-      <c r="N10" s="40"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="13"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="32"/>
       <c r="I11" t="s">
         <v>36</v>
       </c>
       <c r="J11" s="5">
         <v>5.99</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="14">
         <f>J11*E11</f>
         <v>17.97</v>
       </c>
-      <c r="L11" s="41" t="s">
+      <c r="L11" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="36"/>
-      <c r="N11" s="13"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="32"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="2">
-        <v>3</v>
-      </c>
-      <c r="F12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="14"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="4">
         <v>7.99</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="13">
         <f t="shared" ref="K12:K18" si="0">J12*E12</f>
-        <v>23.97</v>
-      </c>
-      <c r="L12" s="42" t="s">
+        <v>7.99</v>
+      </c>
+      <c r="L12" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="14"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="13"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="32"/>
       <c r="J13" s="5">
         <v>9.99</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K13" s="14">
         <f t="shared" si="0"/>
         <v>29.97</v>
       </c>
-      <c r="L13" s="41" t="s">
+      <c r="L13" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="36"/>
-      <c r="N13" s="13"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="32"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="2">
         <v>3</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="8"/>
       <c r="J14" s="4">
         <v>8.2899999999999991</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="13">
         <f t="shared" si="0"/>
         <v>24.869999999999997</v>
       </c>
-      <c r="L14" s="42" t="s">
+      <c r="L14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="31"/>
-      <c r="N14" s="14"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
       <c r="I15" t="s">
         <v>33</v>
       </c>
       <c r="J15" s="5">
         <v>8.69</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="14">
         <f t="shared" si="0"/>
         <v>26.07</v>
       </c>
-      <c r="L15" s="41" t="s">
+      <c r="L15" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="36"/>
-      <c r="N15" s="13"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="32"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="14"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="8"/>
       <c r="J16" s="4">
         <v>6.99</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="13">
         <f t="shared" si="0"/>
-        <v>20.97</v>
-      </c>
-      <c r="L16" s="42" t="s">
+        <v>13.98</v>
+      </c>
+      <c r="L16" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="31"/>
-      <c r="N16" s="14"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="31"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="1">
-        <v>3</v>
-      </c>
-      <c r="F17" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="9"/>
       <c r="J17" s="5">
         <v>11.99</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="14">
         <f t="shared" si="0"/>
-        <v>35.97</v>
-      </c>
-      <c r="L17" s="41" t="s">
+        <v>11.99</v>
+      </c>
+      <c r="L17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="36"/>
-      <c r="N17" s="13"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="32"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="2">
         <v>3</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="31"/>
       <c r="I18" s="8"/>
       <c r="J18" s="4">
         <v>34</v>
       </c>
-      <c r="K18" s="33">
+      <c r="K18" s="13">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="L18" s="42" t="s">
+      <c r="L18" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="31"/>
-      <c r="N18" s="14"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="31"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="18"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="13"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="32"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="13"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="32"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="17"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="14"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="8"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B21" s="18"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="13"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="32"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="13"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="32"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="17"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="14"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="8"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="14"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="31"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="18"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="13"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="32"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="13"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="32"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="17"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="14"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="8"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="14"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="31"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="18"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="13"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="32"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="13"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="32"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="17"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="14"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="8"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="14"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="31"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="18"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="13"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="32"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="13"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="32"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="17"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="14"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="8"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="14"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="31"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="18"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="13"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="32"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="13"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="32"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="19"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="14"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="10"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="16"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="40"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H31" s="32"/>
-      <c r="I31" s="30" t="s">
+      <c r="H31" s="12"/>
+      <c r="I31" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K31" s="7">
         <f>SUM(K10:K30)</f>
-        <v>297.77999999999997</v>
+        <v>250.82999999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="A1:E5"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="L8:N9"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B10:D10"/>
@@ -1344,54 +1383,13 @@
     <mergeCell ref="L18:N18"/>
     <mergeCell ref="L19:N19"/>
     <mergeCell ref="L20:N20"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="A1:E5"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L18" r:id="rId1" xr:uid="{883A45C4-C90C-8F4F-B1E4-9DE9323FF356}"/>

</xml_diff>